<commit_message>
Ajout du plantuml des ressources, mise à jour des descriptions des profils et mise à jour de la page index (#67)
* update deps

* generate intended recipient extension

* change file name

* rm unused aliases

* updat edeps

* adapt to new FrCore

* update status to trial-use

* correct sdemey comments

* clean urls

* update authororg sp

* update links

* update sp isArchives

* rm canonical url

* add file and change names

* update index

* update request template

* update index.md

* update descr

* update index page

* update index page

* update download page

* rm url ea0df281c5c541fc1edca1f5eae3e50ef7fb025b
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-pdsm-find-lists-response.xlsx
+++ b/main/ig/StructureDefinition-pdsm-find-lists-response.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-03T07:57:36+00:00</t>
+    <t>2024-05-28T08:41:18+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -75,7 +75,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Réponse de la transaction IHE "Find Document Lists [ITI-66]" basée sur le bundle MHD http://profiles.ihe.net/ITI/MHD/StructureDefinition/IHE.MHD.FindDocumentListsResponseMessage et profilé pour le volet PDSm</t>
+    <t>Profil de réponse de la transaction IHE "Find Document Lists [ITI-66]" basée sur le bundle MHD FindDocumentListsResponseMessage et profilé pour le volet PDSm</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>